<commit_message>
28th commit: registration date and is admin approved filed added to users class and masterdashboard nested master page created
</commit_message>
<xml_diff>
--- a/OnlineBudgetAnalysisApp/UI/uploads/Inventory.xlsx
+++ b/OnlineBudgetAnalysisApp/UI/uploads/Inventory.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MINHAZ\Desktop\partially final\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MINHAZ\Desktop\Upload\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -381,7 +381,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,10 +405,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C2">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -417,10 +417,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C3">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -429,10 +429,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C4">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -441,10 +441,10 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C5">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -453,10 +453,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -477,10 +477,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C8">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -501,10 +501,10 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C10">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1"/>
     </row>

</xml_diff>

<commit_message>
53th commit: gap problem in datewise report and projectwise report have been fixed
</commit_message>
<xml_diff>
--- a/OnlineBudgetAnalysisApp/UI/uploads/Inventory.xlsx
+++ b/OnlineBudgetAnalysisApp/UI/uploads/Inventory.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MINHAZ\Desktop\Upload\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MINHAZ\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>SKU</t>
   </si>
@@ -36,30 +36,6 @@
   </si>
   <si>
     <t>SKU101</t>
-  </si>
-  <si>
-    <t>SKU102</t>
-  </si>
-  <si>
-    <t>SKU103</t>
-  </si>
-  <si>
-    <t>SKU104</t>
-  </si>
-  <si>
-    <t>SKU105</t>
-  </si>
-  <si>
-    <t>SKU106</t>
-  </si>
-  <si>
-    <t>SKU107</t>
-  </si>
-  <si>
-    <t>SKU108</t>
-  </si>
-  <si>
-    <t>SKU109</t>
   </si>
 </sst>
 </file>
@@ -381,7 +357,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,99 +389,27 @@
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>25</v>
-      </c>
-      <c r="C3">
-        <v>20</v>
-      </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>35</v>
-      </c>
-      <c r="C4">
-        <v>49</v>
-      </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>50</v>
-      </c>
-      <c r="C5">
-        <v>152</v>
-      </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>15</v>
-      </c>
-      <c r="C6">
-        <v>12</v>
-      </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>25</v>
-      </c>
-      <c r="C7">
-        <v>78</v>
-      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>34</v>
-      </c>
-      <c r="C8">
-        <v>444</v>
-      </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>45</v>
-      </c>
-      <c r="C9">
-        <v>282</v>
-      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10">
-        <v>50</v>
-      </c>
-      <c r="C10">
-        <v>40</v>
-      </c>
       <c r="D10" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
57th commit: final commit
</commit_message>
<xml_diff>
--- a/OnlineBudgetAnalysisApp/UI/uploads/Inventory.xlsx
+++ b/OnlineBudgetAnalysisApp/UI/uploads/Inventory.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MINHAZ\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MINHAZ\Desktop\Upload\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>SKU</t>
   </si>
@@ -36,6 +36,30 @@
   </si>
   <si>
     <t>SKU101</t>
+  </si>
+  <si>
+    <t>SKU102</t>
+  </si>
+  <si>
+    <t>SKU103</t>
+  </si>
+  <si>
+    <t>SKU104</t>
+  </si>
+  <si>
+    <t>SKU105</t>
+  </si>
+  <si>
+    <t>SKU106</t>
+  </si>
+  <si>
+    <t>SKU107</t>
+  </si>
+  <si>
+    <t>SKU108</t>
+  </si>
+  <si>
+    <t>SKU109</t>
   </si>
 </sst>
 </file>
@@ -357,7 +381,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,35 +405,107 @@
         <v>3</v>
       </c>
       <c r="B2">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
         <v>20</v>
       </c>
-      <c r="C2">
-        <v>28</v>
-      </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>35</v>
+      </c>
+      <c r="C4">
+        <v>49</v>
+      </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>155</v>
+      </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>77</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>33</v>
+      </c>
+      <c r="C8">
+        <v>440</v>
+      </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>35</v>
+      </c>
+      <c r="C9">
+        <v>278</v>
+      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>43</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
   </sheetData>

</xml_diff>